<commit_message>
First cut with expander code. Needs to be tested!
</commit_message>
<xml_diff>
--- a/hodor/Wemos Board Pinning.xlsx
+++ b/hodor/Wemos Board Pinning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Board Pin</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>Sound board drains too much on the 3V3. Needs external 5V source.</t>
+  </si>
+  <si>
+    <t>With Expander</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>Sound-Tx (not used)</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -197,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,6 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +613,7 @@
     <col min="8" max="8" width="91.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -610,8 +626,11 @@
       <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -626,7 +645,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -643,7 +662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -660,7 +679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -678,8 +697,11 @@
       <c r="H5" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -700,8 +722,11 @@
       <c r="H6" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -718,8 +743,11 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -735,8 +763,11 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -752,8 +783,11 @@
       <c r="F9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -774,7 +808,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>3</v>
       </c>
@@ -782,7 +816,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>1</v>
       </c>
@@ -790,12 +824,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H14" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
New versions that work!
</commit_message>
<xml_diff>
--- a/hodor/Wemos Board Pinning.xlsx
+++ b/hodor/Wemos Board Pinning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Board Pin</t>
   </si>
@@ -152,10 +152,13 @@
     <t>SCL</t>
   </si>
   <si>
-    <t>Sound-Tx (not used)</t>
-  </si>
-  <si>
     <t>INT</t>
+  </si>
+  <si>
+    <t>Sound-Tx</t>
+  </si>
+  <si>
+    <t>do not use this pin</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -212,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,13 +236,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,16 +270,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2323345</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>151984</xdr:rowOff>
+      <xdr:colOff>3713995</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>75784</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -287,7 +302,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4514850" y="3486150"/>
+          <a:off x="5905500" y="3219450"/>
           <a:ext cx="6038095" cy="3323809"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -611,6 +626,7 @@
     <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="91.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -626,7 +642,7 @@
       <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -640,8 +656,7 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -693,12 +708,11 @@
       <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I5" t="s">
-        <v>42</v>
+      <c r="I5" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -718,11 +732,10 @@
       <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -743,7 +756,7 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -763,7 +776,7 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -783,8 +796,8 @@
       <c r="F9" t="s">
         <v>14</v>
       </c>
-      <c r="I9" t="s">
-        <v>43</v>
+      <c r="I9" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -803,8 +816,7 @@
       <c r="F10" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -825,63 +837,81 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="10">
         <v>6</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="10">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="D17" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="10">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="10">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="D19" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="10">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="10">
         <v>11</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes when working to extend the range.
</commit_message>
<xml_diff>
--- a/hodor/Wemos Board Pinning.xlsx
+++ b/hodor/Wemos Board Pinning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Board Pin</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>do not use this pin</t>
+  </si>
+  <si>
+    <t>Board programming:</t>
   </si>
 </sst>
 </file>
@@ -270,15 +273,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>3713995</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>189745</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>75784</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -302,8 +305,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5905500" y="3219450"/>
+          <a:off x="8467725" y="3409950"/>
           <a:ext cx="6038095" cy="3323809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9923</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133923</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9388B9EB-E530-403F-B191-C96F611EC886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5391150" y="3448050"/>
+          <a:ext cx="2848373" cy="4105848"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -615,7 +662,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +902,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>33</v>
       </c>
@@ -866,7 +913,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>33</v>
       </c>
@@ -876,8 +923,11 @@
       <c r="D18" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -890,8 +940,9 @@
       <c r="D19" s="10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>33</v>
       </c>
@@ -902,7 +953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="10" t="s">
         <v>33</v>

</xml_diff>